<commit_message>
📝 Auto-save daily meals
</commit_message>
<xml_diff>
--- a/trackers/2025-12.xlsx
+++ b/trackers/2025-12.xlsx
@@ -7,13 +7,17 @@
     <sheet sheetId="1" name="2025-12-03" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="2025-12-04" state="visible" r:id="rId5"/>
     <sheet sheetId="3" name="2025-12-05" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="2025-12-06" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="2025-12-07" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="2025-12-08" state="visible" r:id="rId9"/>
+    <sheet sheetId="7" name="2025-12-09" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="147">
   <si>
     <t>Time</t>
   </si>
@@ -238,6 +242,222 @@
   </si>
   <si>
     <t>📊 Daily Total (18 meals)</t>
+  </si>
+  <si>
+    <t>📅 Saturday, December 6, 2025</t>
+  </si>
+  <si>
+    <t>11:52</t>
+  </si>
+  <si>
+    <t>Paneer Balti</t>
+  </si>
+  <si>
+    <t>11:54</t>
+  </si>
+  <si>
+    <t>Sevia Upma (1 serving)</t>
+  </si>
+  <si>
+    <t>Sugar (0.7x 1 tsp)</t>
+  </si>
+  <si>
+    <t>11:55</t>
+  </si>
+  <si>
+    <t>1 persimmon (1.5x 1 medium)</t>
+  </si>
+  <si>
+    <t>Nut butter (0.33x 1 tbsp)</t>
+  </si>
+  <si>
+    <t>Pitted dates nour (1x 1 piece)</t>
+  </si>
+  <si>
+    <t>Roasted Kala Chana (0.33 servings)</t>
+  </si>
+  <si>
+    <t>Three Bridges Cheddar &amp; Chive Potatoes (0.33x 1 piece)</t>
+  </si>
+  <si>
+    <t>Banana (0.33x 1 large)</t>
+  </si>
+  <si>
+    <t>11:56</t>
+  </si>
+  <si>
+    <t>Whole wheat bread oroweat (0.5x 1 slice)</t>
+  </si>
+  <si>
+    <t>Ghee (1x 1 tsp)</t>
+  </si>
+  <si>
+    <t>Costco Avocado Box (0.25x 1 mini cup)</t>
+  </si>
+  <si>
+    <t>11:57</t>
+  </si>
+  <si>
+    <t>Poha (0.8 servings)</t>
+  </si>
+  <si>
+    <t>Low fat dahi (0.25x 1 cup)</t>
+  </si>
+  <si>
+    <t>11:58</t>
+  </si>
+  <si>
+    <t>Onion Kulcha</t>
+  </si>
+  <si>
+    <t>Dahi Sev puri with less sweet chutney</t>
+  </si>
+  <si>
+    <t>11:59</t>
+  </si>
+  <si>
+    <t>Plain Naan</t>
+  </si>
+  <si>
+    <t>📊 Daily Total (19 meals)</t>
+  </si>
+  <si>
+    <t>📅 Sunday, December 7, 2025</t>
+  </si>
+  <si>
+    <t>11:36</t>
+  </si>
+  <si>
+    <t>Doodh peda (1x 1 piece)</t>
+  </si>
+  <si>
+    <t>Aloo tikki air fried (2x 1 tikki)</t>
+  </si>
+  <si>
+    <t>Homemade tamarind chutney sweet (1x 1 tbsp)</t>
+  </si>
+  <si>
+    <t>11:37</t>
+  </si>
+  <si>
+    <t>Chole Homemade (1.5 servings)</t>
+  </si>
+  <si>
+    <t>Onion (0.125x 1 cup chopped)</t>
+  </si>
+  <si>
+    <t>11:41</t>
+  </si>
+  <si>
+    <t>Onion Upma (0.8 servings)</t>
+  </si>
+  <si>
+    <t>Brown egg (1x 1 large)</t>
+  </si>
+  <si>
+    <t>11:44</t>
+  </si>
+  <si>
+    <t>Protein Puffs (0.5x 1 serving)</t>
+  </si>
+  <si>
+    <t>11:49</t>
+  </si>
+  <si>
+    <t>Bell pepper Salad (1 serving)</t>
+  </si>
+  <si>
+    <t>11:50</t>
+  </si>
+  <si>
+    <t>Low fat dahi (0.16x 1 cup)</t>
+  </si>
+  <si>
+    <t>Palak Paneer (0.8 servings)</t>
+  </si>
+  <si>
+    <t>11:51</t>
+  </si>
+  <si>
+    <t>Suji Halwa Homemade (0.3x 1 serving)</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>📊 Daily Total (17 meals)</t>
+  </si>
+  <si>
+    <t>📅 Monday, December 8, 2025</t>
+  </si>
+  <si>
+    <t>Dosa (1 serving)</t>
+  </si>
+  <si>
+    <t>12:01</t>
+  </si>
+  <si>
+    <t>12:02</t>
+  </si>
+  <si>
+    <t>Spinach Sambar (0.8 servings)</t>
+  </si>
+  <si>
+    <t>Palak Paneer (1 serving)</t>
+  </si>
+  <si>
+    <t>12:03</t>
+  </si>
+  <si>
+    <t>Orgain vegan protein powder (0.8x 1 serving)</t>
+  </si>
+  <si>
+    <t>12:04</t>
+  </si>
+  <si>
+    <t>Roasted Chana (1 serving)</t>
+  </si>
+  <si>
+    <t>12:06</t>
+  </si>
+  <si>
+    <t>Costco roasted mixed nuts (0.6x 1 tbsp)</t>
+  </si>
+  <si>
+    <t>12:07</t>
+  </si>
+  <si>
+    <t>Costco roasted mixed nuts (1x 1 tbsp)</t>
+  </si>
+  <si>
+    <t>📊 Daily Total (15 meals)</t>
+  </si>
+  <si>
+    <t>📅 Tuesday, December 9, 2025</t>
+  </si>
+  <si>
+    <t>11:13</t>
+  </si>
+  <si>
+    <t>11:14</t>
+  </si>
+  <si>
+    <t>11:27</t>
+  </si>
+  <si>
+    <t>Pumpkin chutney (1 serving)</t>
+  </si>
+  <si>
+    <t>12:08</t>
+  </si>
+  <si>
+    <t>12:09</t>
+  </si>
+  <si>
+    <t>Brinjal Sabji (1 serving)</t>
+  </si>
+  <si>
+    <t>📊 Daily Total (10 meals)</t>
   </si>
 </sst>
 </file>
@@ -2396,4 +2616,2448 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="6">
+        <v>350</v>
+      </c>
+      <c r="E4" s="6">
+        <v>13</v>
+      </c>
+      <c r="F4" s="6">
+        <v>48</v>
+      </c>
+      <c r="G4" s="6">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6">
+        <v>7</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="6">
+        <v>202</v>
+      </c>
+      <c r="E5" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>22.3</v>
+      </c>
+      <c r="G5" s="6">
+        <v>9.2</v>
+      </c>
+      <c r="H5" s="6">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6">
+        <v>66</v>
+      </c>
+      <c r="E6" s="6">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="6">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="6">
+        <v>180</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="6">
+        <v>45</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>9</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="6">
+        <v>33</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="G9" s="6">
+        <v>3</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="6">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>6</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="6">
+        <v>85</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="F11" s="6">
+        <v>13.5</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="H11" s="6">
+        <v>3.8</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="6">
+        <v>73</v>
+      </c>
+      <c r="E12" s="6">
+        <v>4</v>
+      </c>
+      <c r="F12" s="6">
+        <v>5.3</v>
+      </c>
+      <c r="G12" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="6">
+        <v>40</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="6">
+        <v>10.2</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="6">
+        <v>55</v>
+      </c>
+      <c r="E14" s="6">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="6">
+        <v>50</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>5</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="6">
+        <v>33</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="G16" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="6">
+        <v>149</v>
+      </c>
+      <c r="E17" s="6">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6">
+        <v>17.7</v>
+      </c>
+      <c r="G17" s="6">
+        <v>7.7</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="6">
+        <v>28</v>
+      </c>
+      <c r="E18" s="6">
+        <v>2</v>
+      </c>
+      <c r="F18" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="6">
+        <v>68</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>9.9</v>
+      </c>
+      <c r="G19" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="6">
+        <v>150</v>
+      </c>
+      <c r="E20" s="6">
+        <v>6</v>
+      </c>
+      <c r="F20" s="6">
+        <v>21</v>
+      </c>
+      <c r="G20" s="6">
+        <v>5</v>
+      </c>
+      <c r="H20" s="6">
+        <v>3</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="6">
+        <v>160</v>
+      </c>
+      <c r="E21" s="6">
+        <v>6</v>
+      </c>
+      <c r="F21" s="6">
+        <v>22</v>
+      </c>
+      <c r="G21" s="6">
+        <v>5</v>
+      </c>
+      <c r="H21" s="6">
+        <v>3</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="6">
+        <v>280</v>
+      </c>
+      <c r="E22" s="6">
+        <v>11</v>
+      </c>
+      <c r="F22" s="6">
+        <v>39</v>
+      </c>
+      <c r="G22" s="6">
+        <v>9</v>
+      </c>
+      <c r="H22" s="6">
+        <v>6</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="8">
+        <v>2037</v>
+      </c>
+      <c r="E24" s="8">
+        <v>66.3</v>
+      </c>
+      <c r="F24" s="8">
+        <v>278.7</v>
+      </c>
+      <c r="G24" s="8">
+        <v>73.4</v>
+      </c>
+      <c r="H24" s="8">
+        <v>41.2</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="6">
+        <v>133</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="F4" s="6">
+        <v>11.2</v>
+      </c>
+      <c r="G4" s="6">
+        <v>7.4</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="6">
+        <v>300</v>
+      </c>
+      <c r="E5" s="6">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6">
+        <v>50</v>
+      </c>
+      <c r="G5" s="6">
+        <v>8</v>
+      </c>
+      <c r="H5" s="6">
+        <v>8</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="6">
+        <v>60</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>20</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="6">
+        <v>461</v>
+      </c>
+      <c r="E7" s="6">
+        <v>21.3</v>
+      </c>
+      <c r="F7" s="6">
+        <v>67.4</v>
+      </c>
+      <c r="G7" s="6">
+        <v>12.9</v>
+      </c>
+      <c r="H7" s="6">
+        <v>13.2</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="6">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="6">
+        <v>160</v>
+      </c>
+      <c r="E9" s="6">
+        <v>7</v>
+      </c>
+      <c r="F9" s="6">
+        <v>45.4</v>
+      </c>
+      <c r="G9" s="6">
+        <v>24.2</v>
+      </c>
+      <c r="H9" s="6">
+        <v>2.2</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="6">
+        <v>70</v>
+      </c>
+      <c r="E10" s="6">
+        <v>6</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="6">
+        <v>52</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6">
+        <v>8</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="6">
+        <v>38</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="F12" s="6">
+        <v>7.6</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="6">
+        <v>78</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6">
+        <v>13.6</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="6">
+        <v>44</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="6">
+        <v>9.7</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="6">
+        <v>18</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="6">
+        <v>205</v>
+      </c>
+      <c r="E16" s="6">
+        <v>17.2</v>
+      </c>
+      <c r="F16" s="6">
+        <v>8.1</v>
+      </c>
+      <c r="G16" s="6">
+        <v>14.6</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="6">
+        <v>110</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="F17" s="6">
+        <v>16.6</v>
+      </c>
+      <c r="G17" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="H17" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="6">
+        <v>30</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="F18" s="6">
+        <v>6</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="6">
+        <v>41</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="6">
+        <v>68</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>9.9</v>
+      </c>
+      <c r="G20" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1876</v>
+      </c>
+      <c r="E22" s="8">
+        <v>83.6</v>
+      </c>
+      <c r="F22" s="8">
+        <v>283.6</v>
+      </c>
+      <c r="G22" s="8">
+        <v>84.7</v>
+      </c>
+      <c r="H22" s="8">
+        <v>34.5</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="6">
+        <v>210</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5.6</v>
+      </c>
+      <c r="F4" s="6">
+        <v>39.3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="6">
+        <v>70</v>
+      </c>
+      <c r="E5" s="6">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6">
+        <v>41</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="6">
+        <v>183</v>
+      </c>
+      <c r="E7" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="F7" s="6">
+        <v>27.8</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6.8</v>
+      </c>
+      <c r="H7" s="6">
+        <v>6.1</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="6">
+        <v>90</v>
+      </c>
+      <c r="E8" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="F8" s="6">
+        <v>12.1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="H8" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="6">
+        <v>256</v>
+      </c>
+      <c r="E9" s="6">
+        <v>21.5</v>
+      </c>
+      <c r="F9" s="6">
+        <v>10.1</v>
+      </c>
+      <c r="G9" s="6">
+        <v>18.3</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="6">
+        <v>78</v>
+      </c>
+      <c r="E10" s="6">
+        <v>3</v>
+      </c>
+      <c r="F10" s="6">
+        <v>13.6</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="6">
+        <v>44</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="F11" s="6">
+        <v>9.7</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="6">
+        <v>36</v>
+      </c>
+      <c r="E12" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="F12" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="6">
+        <v>128</v>
+      </c>
+      <c r="E13" s="6">
+        <v>16.8</v>
+      </c>
+      <c r="F13" s="6">
+        <v>16</v>
+      </c>
+      <c r="G13" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="H13" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="6">
+        <v>210</v>
+      </c>
+      <c r="E14" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="F14" s="6">
+        <v>32.9</v>
+      </c>
+      <c r="G14" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="H14" s="6">
+        <v>6.3</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="6">
+        <v>38</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="F15" s="6">
+        <v>7.6</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="6">
+        <v>310</v>
+      </c>
+      <c r="E16" s="6">
+        <v>8.1</v>
+      </c>
+      <c r="F16" s="6">
+        <v>48.9</v>
+      </c>
+      <c r="G16" s="6">
+        <v>7.6</v>
+      </c>
+      <c r="H16" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="6">
+        <v>27</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1.1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="6">
+        <v>45</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="G18" s="6">
+        <v>4</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1766</v>
+      </c>
+      <c r="E20" s="8">
+        <v>88.5</v>
+      </c>
+      <c r="F20" s="8">
+        <v>230.9</v>
+      </c>
+      <c r="G20" s="8">
+        <v>61.7</v>
+      </c>
+      <c r="H20" s="8">
+        <v>35.2</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="6">
+        <v>210</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5.6</v>
+      </c>
+      <c r="F4" s="6">
+        <v>39.3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="6">
+        <v>70</v>
+      </c>
+      <c r="E5" s="6">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6">
+        <v>41</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="6">
+        <v>67</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>9.6</v>
+      </c>
+      <c r="G7" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="6">
+        <v>27</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1.1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="6">
+        <v>78</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3</v>
+      </c>
+      <c r="F9" s="6">
+        <v>13.6</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="6">
+        <v>44</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="6">
+        <v>9.7</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="6">
+        <v>36</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="F11" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="6">
+        <v>45</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1.1</v>
+      </c>
+      <c r="F12" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="G12" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="H12" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="6">
+        <v>90</v>
+      </c>
+      <c r="E13" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="F13" s="6">
+        <v>12.1</v>
+      </c>
+      <c r="G13" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="H13" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="8">
+        <v>708</v>
+      </c>
+      <c r="E15" s="8">
+        <v>26.7</v>
+      </c>
+      <c r="F15" s="8">
+        <v>100.9</v>
+      </c>
+      <c r="G15" s="8">
+        <v>23.1</v>
+      </c>
+      <c r="H15" s="8">
+        <v>13.6</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>